<commit_message>
First QA for tutorial content
</commit_message>
<xml_diff>
--- a/src/docs/thirdPartyTools/assets/Gruss_RatingsAutomation.xlsx
+++ b/src/docs/thirdPartyTools/assets/Gruss_RatingsAutomation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\latimerb\Documents\Dev\betfair.docs\src\docs\thirdPartyTools\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C1E51F8D-7CBB-47AA-9E9C-ACDB2ACDAA1A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CB4B46B-B44E-4D60-90A0-B113559CC66D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{43E7A59C-3C50-479C-B837-45E07CEB65C6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{43E7A59C-3C50-479C-B837-45E07CEB65C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Market" sheetId="1" r:id="rId1"/>
@@ -2266,7 +2266,7 @@
   <dimension ref="A1:AC50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q5" sqref="Q5"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5453,7 +5453,7 @@
   <dimension ref="A1:F211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6400,7 +6400,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Kelly auto template
</commit_message>
<xml_diff>
--- a/src/docs/thirdPartyTools/assets/Gruss_RatingsAutomation.xlsx
+++ b/src/docs/thirdPartyTools/assets/Gruss_RatingsAutomation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\latimerb\Documents\Dev\betfair.docs\src\docs\thirdPartyTools\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95D719C1-3B78-4F21-9961-D997F1709B11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028F59F4-1637-48B8-9DF5-88E658B37674}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{43E7A59C-3C50-479C-B837-45E07CEB65C6}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{43E7A59C-3C50-479C-B837-45E07CEB65C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Market" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,10 @@
     <definedName name="BACKLAY">SETTINGS!$C$6</definedName>
     <definedName name="InPlay">Market!$E$2</definedName>
     <definedName name="MarketStatus">Market!$F$2</definedName>
-    <definedName name="Overround">Market!$Y$4</definedName>
+    <definedName name="Overround">Market!$Z$4</definedName>
     <definedName name="Ratings">RATINGS!$J:$J</definedName>
     <definedName name="RunnerName">RATINGS!$L:$L</definedName>
+    <definedName name="SelectionID">RATINGS!$G:$G</definedName>
     <definedName name="stake">SETTINGS!$C$3</definedName>
     <definedName name="TimeTillJump">SETTINGS!$C$9</definedName>
     <definedName name="UserOverround">SETTINGS!$C$5</definedName>
@@ -37,7 +38,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -45,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="536">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="536">
   <si>
     <t>Trigger</t>
   </si>
@@ -1619,40 +1622,40 @@
     <t>LAY</t>
   </si>
   <si>
-    <t>5. Smokin Cindy</t>
-  </si>
-  <si>
-    <t>7. Hook Along Mint</t>
-  </si>
-  <si>
-    <t>3. Riverdale Bear</t>
-  </si>
-  <si>
-    <t>8. Breakfast Creek</t>
-  </si>
-  <si>
-    <t>1. Potent</t>
-  </si>
-  <si>
-    <t>2. Cherokee Cat</t>
-  </si>
-  <si>
-    <t>4. Dressed Up</t>
-  </si>
-  <si>
-    <t>6. Go Quantum</t>
-  </si>
-  <si>
-    <t>4. Awesome Shep</t>
-  </si>
-  <si>
-    <t>1. Cawbourne Dolly</t>
-  </si>
-  <si>
-    <t>8. Lektra Rainbow</t>
-  </si>
-  <si>
     <t>Market 1 Seconds until start</t>
+  </si>
+  <si>
+    <t>GCst (AUS) 29th Jan - 14:38 R1 1800m CL3</t>
+  </si>
+  <si>
+    <t>Horse Racing\AUS\GCst (AUS) 29th Jan</t>
+  </si>
+  <si>
+    <t>Balance:</t>
+  </si>
+  <si>
+    <t>Exposure:</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>1. Calibration</t>
+  </si>
+  <si>
+    <t>2. Bullet Shot</t>
+  </si>
+  <si>
+    <t>3. Single Story</t>
+  </si>
+  <si>
+    <t>4. Dramatic Moments</t>
+  </si>
+  <si>
+    <t>5. Jeopardise Me</t>
+  </si>
+  <si>
+    <t>6. Lady Solerno</t>
   </si>
 </sst>
 </file>
@@ -2852,6 +2855,27 @@
         <vertAlign val="baseline"/>
         <color auto="1"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <vertical/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color auto="1"/>
+      </font>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3029,27 +3053,6 @@
         <vertAlign val="baseline"/>
         <color auto="1"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <vertical/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color auto="1"/>
-      </font>
       <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="medium">
@@ -3210,12 +3213,12 @@
     <tableColumn id="1" xr3:uid="{DE76A775-AD20-4F60-9B41-A37C7FFDB442}" name="Column1" dataDxfId="15"/>
     <tableColumn id="2" xr3:uid="{DDB692EE-C54B-41A2-8DFB-48E32EFDCA47}" name="Column2" dataDxfId="14"/>
     <tableColumn id="3" xr3:uid="{45446E7F-5319-46FE-88B1-F91B93A17CC6}" name="Column3" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{43D2C3A4-6216-471F-B886-95B02DF5D758}" name="Column4" dataDxfId="12">
+    <tableColumn id="4" xr3:uid="{43D2C3A4-6216-471F-B886-95B02DF5D758}" name="Column4" dataDxfId="0">
       <calculatedColumnFormula>IF(
     AND(
         OR(
-             AND(BACKLAY="BACK",(F5&gt;(INDEX(Ratings,MATCH(A5,RunnerName,0))))),
-             AND(BACKLAY="LAY",(F5&lt;(INDEX(Ratings,MATCH(A5,RunnerName,0)))))),
+             AND(BACKLAY="BACK",(F5&gt;(INDEX(Ratings,MATCH(Y5,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F5&lt;(INDEX(Ratings,MATCH(Y5,SelectionID,0)))))),
         Overround&lt;UserOverround,
         TimeTillJump&lt;UserTimeTillJump,
          InPlay="Not In Play",
@@ -3224,20 +3227,18 @@
     ""
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{9F529BD6-B6C4-47BD-B907-68891FA47558}" name="Column5" headerRowDxfId="11" dataDxfId="10">
+    <tableColumn id="5" xr3:uid="{9F529BD6-B6C4-47BD-B907-68891FA47558}" name="Column5" headerRowDxfId="12" dataDxfId="11">
       <calculatedColumnFormula>IF(F5=0,"",F5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{58E48E72-992E-4C08-827D-B0EA61BDCB26}" name="Column6" headerRowDxfId="9" dataDxfId="8" dataCellStyle="Normal 2">
+    <tableColumn id="6" xr3:uid="{58E48E72-992E-4C08-827D-B0EA61BDCB26}" name="Column6" headerRowDxfId="10" dataDxfId="9" dataCellStyle="Normal 2">
       <calculatedColumnFormula>IF(A5="","",IF(BACKLAY="BACK", stake/(F5-1),stake*(H5/(H5-1))-stake))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{9AF55648-4BE7-4A9D-A2C1-DBC35FB592AF}" name="Column7" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{CBBBCB87-B8AC-474B-AAA8-D3C462AF7712}" name="Column8" headerRowDxfId="6" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{23C87B71-3219-4F47-8317-DF8002B912AE}" name="Column9" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{4509516A-6E70-462B-8961-3046AD36D5C0}" name="Column10" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{B0A8E436-D699-4298-B258-418E16C3F2A1}" name="Column11" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{D828D602-3A6F-4204-B491-98CE7F14C55B}" name="Column16" headerRowDxfId="1" dataDxfId="0">
-      <calculatedColumnFormula>IFERROR(100/F5,"")</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="7" xr3:uid="{9AF55648-4BE7-4A9D-A2C1-DBC35FB592AF}" name="Column7" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{CBBBCB87-B8AC-474B-AAA8-D3C462AF7712}" name="Column8" headerRowDxfId="7" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{23C87B71-3219-4F47-8317-DF8002B912AE}" name="Column9" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{4509516A-6E70-462B-8961-3046AD36D5C0}" name="Column10" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{B0A8E436-D699-4298-B258-418E16C3F2A1}" name="Column11" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{D828D602-3A6F-4204-B491-98CE7F14C55B}" name="Column16" headerRowDxfId="2" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3541,10 +3542,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A08F2D9-DA50-403D-B394-A291DB24DE89}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:Y50"/>
+  <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Q5" sqref="Q5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3569,9 +3570,13 @@
     <col min="24" max="24" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="D1" s="1">
-        <v>0.62986111111111109</v>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>525</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="F1" t="s">
+        <v>526</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -3582,32 +3587,41 @@
       <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="N1">
-        <v>29202417</v>
-      </c>
       <c r="O1" t="s">
         <v>10</v>
       </c>
       <c r="P1">
-        <v>2707281917</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+        <v>3140057332</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
       <c r="B2">
-        <v>43551.593038923609</v>
+        <v>43859.606504513889</v>
       </c>
       <c r="C2" s="1">
-        <v>0.59303240740740748</v>
+        <v>0.60649305555555555</v>
       </c>
       <c r="D2" s="1">
-        <v>7.6620370370370366E-3</v>
+        <v>3.2291666666666666E-3</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
       </c>
+      <c r="H2" t="s">
+        <v>527</v>
+      </c>
+      <c r="I2">
+        <v>206.62</v>
+      </c>
+      <c r="K2" t="s">
+        <v>528</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
       <c r="M2" t="s">
         <v>13</v>
       </c>
@@ -3618,12 +3632,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>15</v>
       </c>
       <c r="B3">
-        <v>0.22</v>
+        <v>51939.77</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -3643,8 +3657,8 @@
       <c r="I3" t="s">
         <v>32</v>
       </c>
-      <c r="J3">
-        <v>8</v>
+      <c r="J3" t="s">
+        <v>529</v>
       </c>
       <c r="K3" t="s">
         <v>19</v>
@@ -3656,7 +3670,7 @@
         <v>20</v>
       </c>
       <c r="N3">
-        <v>156714751</v>
+        <v>167967940</v>
       </c>
       <c r="O3" t="s">
         <v>21</v>
@@ -3664,11 +3678,11 @@
       <c r="P3">
         <v>6</v>
       </c>
-      <c r="Y3" t="s">
+      <c r="Z3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>22</v>
       </c>
@@ -3729,66 +3743,69 @@
       <c r="X4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" s="20">
-        <f>SUM(Y5:Y50)</f>
-        <v>131.42880785751765</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z4" s="20">
+        <f>SUM(Z5:Z50)</f>
+        <v>101.38446546671007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>524</v>
+        <v>530</v>
       </c>
       <c r="B5" s="41">
-        <v>10.5</v>
+        <v>4</v>
       </c>
       <c r="C5" s="42">
-        <v>2</v>
+        <v>237</v>
       </c>
       <c r="D5" s="33">
-        <v>12.5</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E5" s="34">
-        <v>2</v>
+        <v>223</v>
       </c>
       <c r="F5" s="25">
-        <v>13</v>
+        <v>4.2</v>
       </c>
       <c r="G5" s="26">
-        <v>4</v>
+        <v>39</v>
       </c>
       <c r="H5" s="49">
-        <v>42</v>
+        <v>4.3</v>
       </c>
       <c r="I5" s="50">
-        <v>6</v>
+        <v>49</v>
       </c>
       <c r="J5" s="57">
-        <v>44</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="K5" s="58">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="L5" s="65">
-        <v>55</v>
+        <v>4.5</v>
       </c>
       <c r="M5" s="66">
-        <v>4</v>
+        <v>173</v>
       </c>
       <c r="N5" s="7">
-        <v>12.053000000000001</v>
+        <v>23.256</v>
       </c>
       <c r="O5" s="7">
-        <v>0</v>
+        <v>4.2</v>
       </c>
       <c r="P5" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="7" t="str">
-        <f t="shared" ref="Q5:Q50" si="0">IF(
+        <v>18457.23</v>
+      </c>
+      <c r="Q5" s="7" t="e">
+        <f>IF(
     AND(
         OR(
-             AND(BACKLAY="BACK",(F5&gt;(INDEX(Ratings,MATCH(A5,RunnerName,0))))),
-             AND(BACKLAY="LAY",(F5&lt;(INDEX(Ratings,MATCH(A5,RunnerName,0)))))),
+             AND(BACKLAY="BACK",(F5&gt;(INDEX(Ratings,MATCH(Y5,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F5&lt;(INDEX(Ratings,MATCH(Y5,SelectionID,0)))))),
         Overround&lt;UserOverround,
         TimeTillJump&lt;UserTimeTillJump,
          InPlay="Not In Play",
@@ -3796,15 +3813,15 @@
         BACKLAY,
     ""
 )</f>
-        <v/>
+        <v>#N/A</v>
       </c>
       <c r="R5" s="10">
         <f>IF(F5=0,"",F5)</f>
-        <v>13</v>
+        <v>4.2</v>
       </c>
       <c r="S5" s="81">
-        <f t="shared" ref="S5:S50" si="1">IF(A5="","",IF(BACKLAY="BACK", stake/(F5-1),stake*(H5/(H5-1))-stake))</f>
-        <v>1.6666666666666667</v>
+        <f t="shared" ref="S5:S50" si="0">IF(A5="","",IF(BACKLAY="BACK", stake/(F5-1),stake*(H5/(H5-1))-stake))</f>
+        <v>6.25</v>
       </c>
       <c r="T5" s="7"/>
       <c r="U5" s="9"/>
@@ -3817,71 +3834,85 @@
       <c r="X5" s="7">
         <v>0</v>
       </c>
-      <c r="Y5" s="19">
-        <f t="shared" ref="Y5:Y50" si="2">IFERROR(100/F5,"")</f>
-        <v>7.6923076923076925</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="Y5">
+        <v>3874770</v>
+      </c>
+      <c r="Z5" s="19">
+        <f t="shared" ref="Z5:Z50" si="1">IFERROR(100/F5,"")</f>
+        <v>23.80952380952381</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>525</v>
+        <v>531</v>
       </c>
       <c r="B6" s="43">
-        <v>40</v>
+        <v>6.2</v>
       </c>
       <c r="C6" s="44">
-        <v>8</v>
+        <v>113</v>
       </c>
       <c r="D6" s="35">
-        <v>50</v>
+        <v>6.4</v>
       </c>
       <c r="E6" s="36">
-        <v>10</v>
+        <v>123</v>
       </c>
       <c r="F6" s="27">
-        <v>75</v>
+        <v>6.6</v>
       </c>
       <c r="G6" s="28">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="H6" s="51">
-        <v>1000</v>
+        <v>6.8</v>
       </c>
       <c r="I6" s="52">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="J6" s="59">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="K6" s="60">
-        <v>0</v>
+        <v>72</v>
       </c>
       <c r="L6" s="67">
-        <v>0</v>
+        <v>7.2</v>
       </c>
       <c r="M6" s="68">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="N6" s="7">
-        <v>1.581</v>
+        <v>16.667000000000002</v>
       </c>
       <c r="O6" s="7">
-        <v>0</v>
+        <v>6.6</v>
       </c>
       <c r="P6" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="7" t="str">
+        <v>3274.22</v>
+      </c>
+      <c r="Q6" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F6&gt;(INDEX(Ratings,MATCH(Y6,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F6&lt;(INDEX(Ratings,MATCH(Y6,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R6" s="10">
+        <f t="shared" ref="R6:R50" si="2">IF(F6=0,"",F6)</f>
+        <v>6.6</v>
+      </c>
+      <c r="S6" s="81">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="R6" s="10">
-        <f t="shared" ref="R6:R50" si="3">IF(F6=0,"",F6)</f>
-        <v>75</v>
-      </c>
-      <c r="S6" s="81">
-        <f t="shared" si="1"/>
-        <v>0.27027027027027029</v>
+        <v>3.5714285714285716</v>
       </c>
       <c r="T6" s="7"/>
       <c r="U6" s="9"/>
@@ -3894,71 +3925,85 @@
       <c r="X6" s="7">
         <v>0</v>
       </c>
-      <c r="Y6" s="19">
+      <c r="Y6">
+        <v>20723416</v>
+      </c>
+      <c r="Z6" s="19">
+        <f t="shared" si="1"/>
+        <v>15.151515151515152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>532</v>
+      </c>
+      <c r="B7" s="45">
+        <v>9.4</v>
+      </c>
+      <c r="C7" s="46">
+        <v>28</v>
+      </c>
+      <c r="D7" s="37">
+        <v>9.6</v>
+      </c>
+      <c r="E7" s="38">
+        <v>19</v>
+      </c>
+      <c r="F7" s="29">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="G7" s="30">
+        <v>11</v>
+      </c>
+      <c r="H7" s="53">
+        <v>10</v>
+      </c>
+      <c r="I7" s="54">
+        <v>32</v>
+      </c>
+      <c r="J7" s="61">
+        <v>10.5</v>
+      </c>
+      <c r="K7" s="62">
+        <v>194</v>
+      </c>
+      <c r="L7" s="69">
+        <v>11.5</v>
+      </c>
+      <c r="M7" s="70">
+        <v>10</v>
+      </c>
+      <c r="N7" s="7">
+        <v>11.111000000000001</v>
+      </c>
+      <c r="O7" s="7">
+        <v>9.4</v>
+      </c>
+      <c r="P7" s="7">
+        <v>1593.92</v>
+      </c>
+      <c r="Q7" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F7&gt;(INDEX(Ratings,MATCH(Y7,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F7&lt;(INDEX(Ratings,MATCH(Y7,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R7" s="10">
         <f t="shared" si="2"/>
-        <v>1.3333333333333333</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="12" t="s">
-        <v>526</v>
-      </c>
-      <c r="B7" s="45">
-        <v>18</v>
-      </c>
-      <c r="C7" s="46">
-        <v>4</v>
-      </c>
-      <c r="D7" s="37">
-        <v>19.5</v>
-      </c>
-      <c r="E7" s="38">
-        <v>3</v>
-      </c>
-      <c r="F7" s="29">
-        <v>20</v>
-      </c>
-      <c r="G7" s="30">
-        <v>2</v>
-      </c>
-      <c r="H7" s="53">
-        <v>65</v>
-      </c>
-      <c r="I7" s="54">
-        <v>5</v>
-      </c>
-      <c r="J7" s="61">
-        <v>95</v>
-      </c>
-      <c r="K7" s="62">
-        <v>5</v>
-      </c>
-      <c r="L7" s="69">
-        <v>130</v>
-      </c>
-      <c r="M7" s="70">
-        <v>4</v>
-      </c>
-      <c r="N7" s="7">
-        <v>7.7080000000000002</v>
-      </c>
-      <c r="O7" s="7">
-        <v>0</v>
-      </c>
-      <c r="P7" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="7" t="str">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="S7" s="81">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="R7" s="10">
-        <f t="shared" si="3"/>
-        <v>20</v>
-      </c>
-      <c r="S7" s="81">
-        <f t="shared" si="1"/>
-        <v>1.0526315789473684</v>
+        <v>2.2727272727272725</v>
       </c>
       <c r="T7" s="7"/>
       <c r="U7" s="9"/>
@@ -3971,71 +4016,85 @@
       <c r="X7" s="7">
         <v>0</v>
       </c>
-      <c r="Y7" s="19">
+      <c r="Y7">
+        <v>19842236</v>
+      </c>
+      <c r="Z7" s="19">
+        <f t="shared" si="1"/>
+        <v>10.204081632653061</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="B8" s="43">
+        <v>10</v>
+      </c>
+      <c r="C8" s="44">
+        <v>55</v>
+      </c>
+      <c r="D8" s="35">
+        <v>10.5</v>
+      </c>
+      <c r="E8" s="36">
+        <v>53</v>
+      </c>
+      <c r="F8" s="27">
+        <v>11</v>
+      </c>
+      <c r="G8" s="28">
+        <v>11</v>
+      </c>
+      <c r="H8" s="51">
+        <v>11.5</v>
+      </c>
+      <c r="I8" s="52">
+        <v>38</v>
+      </c>
+      <c r="J8" s="59">
+        <v>12</v>
+      </c>
+      <c r="K8" s="60">
+        <v>28</v>
+      </c>
+      <c r="L8" s="67">
+        <v>12.5</v>
+      </c>
+      <c r="M8" s="68">
+        <v>35</v>
+      </c>
+      <c r="N8" s="7">
+        <v>9.0909999999999993</v>
+      </c>
+      <c r="O8" s="7">
+        <v>11</v>
+      </c>
+      <c r="P8" s="7">
+        <v>5031.28</v>
+      </c>
+      <c r="Q8" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F8&gt;(INDEX(Ratings,MATCH(Y8,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F8&lt;(INDEX(Ratings,MATCH(Y8,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R8" s="10">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>527</v>
-      </c>
-      <c r="B8" s="43">
-        <v>1.76</v>
-      </c>
-      <c r="C8" s="44">
-        <v>18</v>
-      </c>
-      <c r="D8" s="35">
-        <v>1.77</v>
-      </c>
-      <c r="E8" s="36">
-        <v>3</v>
-      </c>
-      <c r="F8" s="27">
-        <v>1.78</v>
-      </c>
-      <c r="G8" s="28">
-        <v>3</v>
-      </c>
-      <c r="H8" s="51">
-        <v>2.08</v>
-      </c>
-      <c r="I8" s="52">
-        <v>4</v>
-      </c>
-      <c r="J8" s="59">
-        <v>2.98</v>
-      </c>
-      <c r="K8" s="60">
-        <v>9</v>
-      </c>
-      <c r="L8" s="67">
-        <v>3.05</v>
-      </c>
-      <c r="M8" s="68">
-        <v>162</v>
-      </c>
-      <c r="N8" s="7">
-        <v>34.783000000000001</v>
-      </c>
-      <c r="O8" s="7">
-        <v>0</v>
-      </c>
-      <c r="P8" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="7" t="str">
+        <v>11</v>
+      </c>
+      <c r="S8" s="81">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="R8" s="10">
-        <f t="shared" si="3"/>
-        <v>1.78</v>
-      </c>
-      <c r="S8" s="81">
-        <f t="shared" si="1"/>
-        <v>25.641025641025639</v>
+        <v>2</v>
       </c>
       <c r="T8" s="7"/>
       <c r="U8" s="9"/>
@@ -4048,71 +4107,85 @@
       <c r="X8" s="7">
         <v>0</v>
       </c>
-      <c r="Y8" s="19">
+      <c r="Y8">
+        <v>2095049</v>
+      </c>
+      <c r="Z8" s="19">
+        <f t="shared" si="1"/>
+        <v>9.0909090909090917</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="12" t="s">
+        <v>534</v>
+      </c>
+      <c r="B9" s="45">
+        <v>2.72</v>
+      </c>
+      <c r="C9" s="46">
+        <v>111</v>
+      </c>
+      <c r="D9" s="37">
+        <v>2.74</v>
+      </c>
+      <c r="E9" s="38">
+        <v>9</v>
+      </c>
+      <c r="F9" s="29">
+        <v>2.76</v>
+      </c>
+      <c r="G9" s="30">
+        <v>11</v>
+      </c>
+      <c r="H9" s="53">
+        <v>2.78</v>
+      </c>
+      <c r="I9" s="54">
+        <v>56</v>
+      </c>
+      <c r="J9" s="61">
+        <v>2.8</v>
+      </c>
+      <c r="K9" s="62">
+        <v>55</v>
+      </c>
+      <c r="L9" s="69">
+        <v>2.82</v>
+      </c>
+      <c r="M9" s="70">
+        <v>242</v>
+      </c>
+      <c r="N9" s="7">
+        <v>32.975000000000001</v>
+      </c>
+      <c r="O9" s="7">
+        <v>2.74</v>
+      </c>
+      <c r="P9" s="7">
+        <v>21737.200000000001</v>
+      </c>
+      <c r="Q9" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F9&gt;(INDEX(Ratings,MATCH(Y9,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F9&lt;(INDEX(Ratings,MATCH(Y9,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R9" s="10">
         <f t="shared" si="2"/>
-        <v>56.179775280898873</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
-        <v>528</v>
-      </c>
-      <c r="B9" s="45">
-        <v>5.8</v>
-      </c>
-      <c r="C9" s="46">
-        <v>4</v>
-      </c>
-      <c r="D9" s="37">
-        <v>5.9</v>
-      </c>
-      <c r="E9" s="38">
-        <v>5</v>
-      </c>
-      <c r="F9" s="29">
-        <v>6</v>
-      </c>
-      <c r="G9" s="30">
-        <v>15</v>
-      </c>
-      <c r="H9" s="53">
-        <v>14.5</v>
-      </c>
-      <c r="I9" s="54">
-        <v>2</v>
-      </c>
-      <c r="J9" s="61">
-        <v>15</v>
-      </c>
-      <c r="K9" s="62">
-        <v>4</v>
-      </c>
-      <c r="L9" s="69">
-        <v>15.5</v>
-      </c>
-      <c r="M9" s="70">
-        <v>22</v>
-      </c>
-      <c r="N9" s="7">
-        <v>7.7080000000000002</v>
-      </c>
-      <c r="O9" s="7">
-        <v>0</v>
-      </c>
-      <c r="P9" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="7" t="str">
+        <v>2.76</v>
+      </c>
+      <c r="S9" s="81">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="R9" s="10">
-        <f t="shared" si="3"/>
-        <v>6</v>
-      </c>
-      <c r="S9" s="81">
-        <f t="shared" si="1"/>
-        <v>4</v>
+        <v>11.363636363636365</v>
       </c>
       <c r="T9" s="7"/>
       <c r="U9" s="9"/>
@@ -4125,71 +4198,85 @@
       <c r="X9" s="7">
         <v>0</v>
       </c>
-      <c r="Y9" s="19">
+      <c r="Y9">
+        <v>27673254</v>
+      </c>
+      <c r="Z9" s="19">
+        <f t="shared" si="1"/>
+        <v>36.231884057971016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>535</v>
+      </c>
+      <c r="B10" s="43">
+        <v>13.5</v>
+      </c>
+      <c r="C10" s="44">
+        <v>149</v>
+      </c>
+      <c r="D10" s="35">
+        <v>14</v>
+      </c>
+      <c r="E10" s="36">
+        <v>89</v>
+      </c>
+      <c r="F10" s="27">
+        <v>14.5</v>
+      </c>
+      <c r="G10" s="28">
+        <v>23</v>
+      </c>
+      <c r="H10" s="51">
+        <v>15</v>
+      </c>
+      <c r="I10" s="52">
+        <v>17</v>
+      </c>
+      <c r="J10" s="59">
+        <v>15.5</v>
+      </c>
+      <c r="K10" s="60">
+        <v>47</v>
+      </c>
+      <c r="L10" s="67">
+        <v>16</v>
+      </c>
+      <c r="M10" s="68">
+        <v>168</v>
+      </c>
+      <c r="N10" s="7">
+        <v>6.9</v>
+      </c>
+      <c r="O10" s="7">
+        <v>15</v>
+      </c>
+      <c r="P10" s="7">
+        <v>1845.93</v>
+      </c>
+      <c r="Q10" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F10&gt;(INDEX(Ratings,MATCH(Y10,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F10&lt;(INDEX(Ratings,MATCH(Y10,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R10" s="10">
         <f t="shared" si="2"/>
-        <v>16.666666666666668</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>529</v>
-      </c>
-      <c r="B10" s="43">
-        <v>100</v>
-      </c>
-      <c r="C10" s="44">
-        <v>5</v>
-      </c>
-      <c r="D10" s="35">
-        <v>110</v>
-      </c>
-      <c r="E10" s="36">
-        <v>2</v>
-      </c>
-      <c r="F10" s="27">
-        <v>300</v>
-      </c>
-      <c r="G10" s="28">
-        <v>9</v>
-      </c>
-      <c r="H10" s="51">
-        <v>600</v>
-      </c>
-      <c r="I10" s="52">
-        <v>4</v>
-      </c>
-      <c r="J10" s="59">
-        <v>1000</v>
-      </c>
-      <c r="K10" s="60">
-        <v>2</v>
-      </c>
-      <c r="L10" s="67">
-        <v>0</v>
-      </c>
-      <c r="M10" s="68">
-        <v>0</v>
-      </c>
-      <c r="N10" s="7">
-        <v>1.581</v>
-      </c>
-      <c r="O10" s="7">
-        <v>150</v>
-      </c>
-      <c r="P10" s="7">
-        <v>0.11</v>
-      </c>
-      <c r="Q10" s="7" t="str">
+        <v>14.5</v>
+      </c>
+      <c r="S10" s="81">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="R10" s="10">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-      <c r="S10" s="81">
-        <f t="shared" si="1"/>
-        <v>6.6889632107023408E-2</v>
+        <v>1.4814814814814814</v>
       </c>
       <c r="T10" s="7"/>
       <c r="U10" s="9"/>
@@ -4202,71 +4289,53 @@
       <c r="X10" s="7">
         <v>0</v>
       </c>
-      <c r="Y10" s="19">
+      <c r="Y10">
+        <v>20385931</v>
+      </c>
+      <c r="Z10" s="19">
+        <f t="shared" si="1"/>
+        <v>6.8965517241379306</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="12"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="29"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="70"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F11&gt;(INDEX(Ratings,MATCH(Y11,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F11&lt;(INDEX(Ratings,MATCH(Y11,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R11" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>0.33333333333333331</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="12" t="s">
-        <v>530</v>
-      </c>
-      <c r="B11" s="45">
-        <v>9.4</v>
-      </c>
-      <c r="C11" s="46">
-        <v>39</v>
-      </c>
-      <c r="D11" s="37">
-        <v>9.6</v>
-      </c>
-      <c r="E11" s="38">
-        <v>4</v>
-      </c>
-      <c r="F11" s="29">
-        <v>10.5</v>
-      </c>
-      <c r="G11" s="30">
-        <v>5</v>
-      </c>
-      <c r="H11" s="53">
-        <v>12</v>
-      </c>
-      <c r="I11" s="54">
-        <v>5</v>
-      </c>
-      <c r="J11" s="61">
-        <v>17.5</v>
-      </c>
-      <c r="K11" s="62">
-        <v>4</v>
-      </c>
-      <c r="L11" s="69">
-        <v>21</v>
-      </c>
-      <c r="M11" s="70">
-        <v>5</v>
-      </c>
-      <c r="N11" s="7">
-        <v>12.834</v>
-      </c>
-      <c r="O11" s="7">
-        <v>0</v>
-      </c>
-      <c r="P11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S11" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
-      </c>
-      <c r="R11" s="10">
-        <f t="shared" si="3"/>
-        <v>10.5</v>
-      </c>
-      <c r="S11" s="81">
-        <f t="shared" si="1"/>
-        <v>2.1052631578947367</v>
       </c>
       <c r="T11" s="7"/>
       <c r="U11" s="9"/>
@@ -4276,74 +4345,51 @@
       <c r="W11" s="7">
         <v>0</v>
       </c>
-      <c r="X11" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="19">
+      <c r="X11" s="7"/>
+      <c r="Z11" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="12"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="44"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="51"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="60"/>
+      <c r="L12" s="67"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F12&gt;(INDEX(Ratings,MATCH(Y12,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F12&lt;(INDEX(Ratings,MATCH(Y12,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R12" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>9.5238095238095237</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
-        <v>531</v>
-      </c>
-      <c r="B12" s="43">
-        <v>75</v>
-      </c>
-      <c r="C12" s="44">
-        <v>7</v>
-      </c>
-      <c r="D12" s="35">
-        <v>100</v>
-      </c>
-      <c r="E12" s="36">
-        <v>5</v>
-      </c>
-      <c r="F12" s="27">
-        <v>110</v>
-      </c>
-      <c r="G12" s="28">
-        <v>2</v>
-      </c>
-      <c r="H12" s="51">
-        <v>590</v>
-      </c>
-      <c r="I12" s="52">
-        <v>4</v>
-      </c>
-      <c r="J12" s="59">
-        <v>1000</v>
-      </c>
-      <c r="K12" s="60">
-        <v>2</v>
-      </c>
-      <c r="L12" s="67">
-        <v>0</v>
-      </c>
-      <c r="M12" s="68">
-        <v>0</v>
-      </c>
-      <c r="N12" s="7">
-        <v>0.85199999999999998</v>
-      </c>
-      <c r="O12" s="7">
-        <v>150</v>
-      </c>
-      <c r="P12" s="7">
-        <v>0.11</v>
-      </c>
-      <c r="Q12" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S12" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
-      </c>
-      <c r="R12" s="10">
-        <f t="shared" si="3"/>
-        <v>110</v>
-      </c>
-      <c r="S12" s="81">
-        <f t="shared" si="1"/>
-        <v>0.1834862385321101</v>
       </c>
       <c r="T12" s="7"/>
       <c r="U12" s="9"/>
@@ -4353,74 +4399,51 @@
       <c r="W12" s="7">
         <v>0</v>
       </c>
-      <c r="X12" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="19">
-        <f t="shared" si="2"/>
-        <v>0.90909090909090906</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>532</v>
-      </c>
-      <c r="B13" s="45">
-        <v>4.2</v>
-      </c>
-      <c r="C13" s="46">
-        <v>14</v>
-      </c>
-      <c r="D13" s="37">
-        <v>4.3</v>
-      </c>
-      <c r="E13" s="38">
-        <v>8</v>
-      </c>
-      <c r="F13" s="29">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="G13" s="30">
-        <v>8</v>
-      </c>
-      <c r="H13" s="53">
-        <v>5.9</v>
-      </c>
-      <c r="I13" s="54">
-        <v>5</v>
-      </c>
-      <c r="J13" s="61">
-        <v>6</v>
-      </c>
-      <c r="K13" s="62">
-        <v>5</v>
-      </c>
-      <c r="L13" s="69">
-        <v>8.6</v>
-      </c>
-      <c r="M13" s="70">
-        <v>45</v>
-      </c>
-      <c r="N13" s="7">
-        <v>6.1619999999999999</v>
-      </c>
-      <c r="O13" s="7">
-        <v>0</v>
-      </c>
-      <c r="P13" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="7" t="str">
+      <c r="X12" s="7"/>
+      <c r="Z12" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="12"/>
+      <c r="B13" s="45"/>
+      <c r="C13" s="46"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="29"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="70"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F13&gt;(INDEX(Ratings,MATCH(Y13,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F13&lt;(INDEX(Ratings,MATCH(Y13,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R13" s="10" t="str">
+        <f>IF(F13=0,"",F13)</f>
+        <v/>
+      </c>
+      <c r="S13" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
-      </c>
-      <c r="R13" s="10">
-        <f>IF(F13=0,"",F13)</f>
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="S13" s="81">
-        <f t="shared" si="1"/>
-        <v>5.8823529411764701</v>
       </c>
       <c r="T13" s="7"/>
       <c r="U13" s="7"/>
@@ -4430,74 +4453,51 @@
       <c r="W13" s="7">
         <v>0</v>
       </c>
-      <c r="X13" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="19">
+      <c r="X13" s="7"/>
+      <c r="Z13" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="12"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="59"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="67"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F14&gt;(INDEX(Ratings,MATCH(Y14,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F14&lt;(INDEX(Ratings,MATCH(Y14,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R14" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>22.727272727272727</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>533</v>
-      </c>
-      <c r="B14" s="43">
-        <v>10</v>
-      </c>
-      <c r="C14" s="44">
-        <v>4</v>
-      </c>
-      <c r="D14" s="35">
-        <v>13.5</v>
-      </c>
-      <c r="E14" s="36">
-        <v>3</v>
-      </c>
-      <c r="F14" s="27">
-        <v>14.5</v>
-      </c>
-      <c r="G14" s="28">
-        <v>3</v>
-      </c>
-      <c r="H14" s="51">
-        <v>26</v>
-      </c>
-      <c r="I14" s="52">
-        <v>2</v>
-      </c>
-      <c r="J14" s="59">
-        <v>32</v>
-      </c>
-      <c r="K14" s="60">
-        <v>4</v>
-      </c>
-      <c r="L14" s="67">
-        <v>44</v>
-      </c>
-      <c r="M14" s="68">
-        <v>7</v>
-      </c>
-      <c r="N14" s="7">
-        <v>10.173999999999999</v>
-      </c>
-      <c r="O14" s="7">
-        <v>0</v>
-      </c>
-      <c r="P14" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S14" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
-      </c>
-      <c r="R14" s="10">
-        <f t="shared" si="3"/>
-        <v>14.5</v>
-      </c>
-      <c r="S14" s="81">
-        <f t="shared" si="1"/>
-        <v>1.4814814814814814</v>
       </c>
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
@@ -4507,74 +4507,51 @@
       <c r="W14" s="7">
         <v>0</v>
       </c>
-      <c r="X14" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="19">
+      <c r="X14" s="7"/>
+      <c r="Z14" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="12"/>
+      <c r="B15" s="45"/>
+      <c r="C15" s="46"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="29"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="70"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F15&gt;(INDEX(Ratings,MATCH(Y15,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F15&lt;(INDEX(Ratings,MATCH(Y15,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R15" s="10" t="str">
         <f t="shared" si="2"/>
-        <v>6.8965517241379306</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>534</v>
-      </c>
-      <c r="B15" s="45">
-        <v>22</v>
-      </c>
-      <c r="C15" s="46">
-        <v>4</v>
-      </c>
-      <c r="D15" s="37">
-        <v>23</v>
-      </c>
-      <c r="E15" s="38">
-        <v>4</v>
-      </c>
-      <c r="F15" s="29">
-        <v>24</v>
-      </c>
-      <c r="G15" s="30">
-        <v>2</v>
-      </c>
-      <c r="H15" s="53">
-        <v>130</v>
-      </c>
-      <c r="I15" s="54">
-        <v>5</v>
-      </c>
-      <c r="J15" s="61">
-        <v>180</v>
-      </c>
-      <c r="K15" s="62">
-        <v>5</v>
-      </c>
-      <c r="L15" s="69">
-        <v>220</v>
-      </c>
-      <c r="M15" s="70">
-        <v>4</v>
-      </c>
-      <c r="N15" s="7">
-        <v>4.5629999999999997</v>
-      </c>
-      <c r="O15" s="7">
-        <v>0</v>
-      </c>
-      <c r="P15" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="7" t="str">
+        <v/>
+      </c>
+      <c r="S15" s="81" t="str">
         <f t="shared" si="0"/>
         <v/>
-      </c>
-      <c r="R15" s="10">
-        <f t="shared" si="3"/>
-        <v>24</v>
-      </c>
-      <c r="S15" s="81">
-        <f t="shared" si="1"/>
-        <v>0.86956521739130432</v>
       </c>
       <c r="T15" s="7"/>
       <c r="U15" s="7"/>
@@ -4584,15 +4561,13 @@
       <c r="W15" s="7">
         <v>0</v>
       </c>
-      <c r="X15" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="19">
-        <f t="shared" si="2"/>
-        <v>4.166666666666667</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="X15" s="7"/>
+      <c r="Z15" s="19" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
       <c r="B16" s="43"/>
       <c r="C16" s="44"/>
@@ -4610,15 +4585,26 @@
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
       <c r="Q16" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F16&gt;(INDEX(Ratings,MATCH(Y16,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F16&lt;(INDEX(Ratings,MATCH(Y16,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R16" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S16" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R16" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S16" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T16" s="7"/>
@@ -4626,12 +4612,12 @@
       <c r="V16" s="7"/>
       <c r="W16" s="7"/>
       <c r="X16" s="7"/>
-      <c r="Y16" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z16" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="45"/>
       <c r="C17" s="46"/>
@@ -4649,15 +4635,26 @@
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
       <c r="Q17" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F17&gt;(INDEX(Ratings,MATCH(Y17,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F17&lt;(INDEX(Ratings,MATCH(Y17,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R17" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S17" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R17" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S17" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T17" s="7"/>
@@ -4665,12 +4662,12 @@
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
       <c r="X17" s="7"/>
-      <c r="Y17" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z17" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="43"/>
       <c r="C18" s="44"/>
@@ -4688,15 +4685,26 @@
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
       <c r="Q18" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F18&gt;(INDEX(Ratings,MATCH(Y18,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F18&lt;(INDEX(Ratings,MATCH(Y18,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R18" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S18" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R18" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S18" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T18" s="7"/>
@@ -4704,12 +4712,12 @@
       <c r="V18" s="7"/>
       <c r="W18" s="7"/>
       <c r="X18" s="7"/>
-      <c r="Y18" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z18" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="45"/>
       <c r="C19" s="46"/>
@@ -4727,15 +4735,26 @@
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
       <c r="Q19" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F19&gt;(INDEX(Ratings,MATCH(Y19,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F19&lt;(INDEX(Ratings,MATCH(Y19,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R19" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S19" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R19" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S19" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T19" s="7"/>
@@ -4743,12 +4762,12 @@
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
-      <c r="Y19" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z19" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="43"/>
       <c r="C20" s="44"/>
@@ -4766,15 +4785,26 @@
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
       <c r="Q20" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F20&gt;(INDEX(Ratings,MATCH(Y20,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F20&lt;(INDEX(Ratings,MATCH(Y20,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R20" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S20" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R20" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S20" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T20" s="7"/>
@@ -4782,12 +4812,12 @@
       <c r="V20" s="7"/>
       <c r="W20" s="7"/>
       <c r="X20" s="7"/>
-      <c r="Y20" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z20" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="45"/>
       <c r="C21" s="46"/>
@@ -4805,15 +4835,26 @@
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
       <c r="Q21" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F21&gt;(INDEX(Ratings,MATCH(Y21,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F21&lt;(INDEX(Ratings,MATCH(Y21,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R21" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S21" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R21" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S21" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T21" s="7"/>
@@ -4821,12 +4862,12 @@
       <c r="V21" s="7"/>
       <c r="W21" s="7"/>
       <c r="X21" s="7"/>
-      <c r="Y21" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z21" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="43"/>
       <c r="C22" s="44"/>
@@ -4844,15 +4885,26 @@
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
       <c r="Q22" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F22&gt;(INDEX(Ratings,MATCH(Y22,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F22&lt;(INDEX(Ratings,MATCH(Y22,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R22" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S22" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R22" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S22" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T22" s="7"/>
@@ -4860,12 +4912,12 @@
       <c r="V22" s="7"/>
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
-      <c r="Y22" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z22" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="45"/>
       <c r="C23" s="46"/>
@@ -4883,15 +4935,26 @@
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
       <c r="Q23" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F23&gt;(INDEX(Ratings,MATCH(Y23,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F23&lt;(INDEX(Ratings,MATCH(Y23,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R23" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S23" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R23" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S23" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T23" s="7"/>
@@ -4899,12 +4962,12 @@
       <c r="V23" s="7"/>
       <c r="W23" s="7"/>
       <c r="X23" s="7"/>
-      <c r="Y23" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z23" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="43"/>
       <c r="C24" s="44"/>
@@ -4922,15 +4985,26 @@
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
       <c r="Q24" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F24&gt;(INDEX(Ratings,MATCH(Y24,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F24&lt;(INDEX(Ratings,MATCH(Y24,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R24" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S24" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R24" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S24" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T24" s="7"/>
@@ -4938,12 +5012,12 @@
       <c r="V24" s="7"/>
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
-      <c r="Y24" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z24" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="45"/>
       <c r="C25" s="46"/>
@@ -4961,15 +5035,26 @@
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
       <c r="Q25" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F25&gt;(INDEX(Ratings,MATCH(Y25,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F25&lt;(INDEX(Ratings,MATCH(Y25,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R25" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S25" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R25" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S25" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T25" s="7"/>
@@ -4977,12 +5062,12 @@
       <c r="V25" s="7"/>
       <c r="W25" s="7"/>
       <c r="X25" s="7"/>
-      <c r="Y25" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z25" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="B26" s="43"/>
       <c r="C26" s="44"/>
@@ -5000,15 +5085,26 @@
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
       <c r="Q26" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F26&gt;(INDEX(Ratings,MATCH(Y26,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F26&lt;(INDEX(Ratings,MATCH(Y26,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R26" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S26" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R26" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S26" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T26" s="7"/>
@@ -5016,12 +5112,12 @@
       <c r="V26" s="7"/>
       <c r="W26" s="7"/>
       <c r="X26" s="7"/>
-      <c r="Y26" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z26" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="45"/>
       <c r="C27" s="46"/>
@@ -5039,15 +5135,26 @@
       <c r="O27" s="7"/>
       <c r="P27" s="7"/>
       <c r="Q27" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F27&gt;(INDEX(Ratings,MATCH(Y27,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F27&lt;(INDEX(Ratings,MATCH(Y27,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R27" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S27" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R27" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S27" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T27" s="7"/>
@@ -5055,12 +5162,12 @@
       <c r="V27" s="7"/>
       <c r="W27" s="7"/>
       <c r="X27" s="7"/>
-      <c r="Y27" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z27" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="43"/>
       <c r="C28" s="44"/>
@@ -5078,15 +5185,26 @@
       <c r="O28" s="7"/>
       <c r="P28" s="7"/>
       <c r="Q28" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F28&gt;(INDEX(Ratings,MATCH(Y28,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F28&lt;(INDEX(Ratings,MATCH(Y28,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R28" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S28" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R28" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S28" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T28" s="7"/>
@@ -5094,12 +5212,12 @@
       <c r="V28" s="7"/>
       <c r="W28" s="7"/>
       <c r="X28" s="7"/>
-      <c r="Y28" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z28" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="B29" s="45"/>
       <c r="C29" s="46"/>
@@ -5117,15 +5235,26 @@
       <c r="O29" s="7"/>
       <c r="P29" s="7"/>
       <c r="Q29" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F29&gt;(INDEX(Ratings,MATCH(Y29,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F29&lt;(INDEX(Ratings,MATCH(Y29,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R29" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S29" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R29" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S29" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T29" s="7"/>
@@ -5133,12 +5262,12 @@
       <c r="V29" s="7"/>
       <c r="W29" s="7"/>
       <c r="X29" s="7"/>
-      <c r="Y29" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z29" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="43"/>
       <c r="C30" s="44"/>
@@ -5156,15 +5285,26 @@
       <c r="O30" s="7"/>
       <c r="P30" s="7"/>
       <c r="Q30" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F30&gt;(INDEX(Ratings,MATCH(Y30,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F30&lt;(INDEX(Ratings,MATCH(Y30,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R30" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S30" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R30" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S30" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T30" s="7"/>
@@ -5172,12 +5312,12 @@
       <c r="V30" s="7"/>
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
-      <c r="Y30" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z30" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="45"/>
       <c r="C31" s="46"/>
@@ -5195,15 +5335,26 @@
       <c r="O31" s="7"/>
       <c r="P31" s="7"/>
       <c r="Q31" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F31&gt;(INDEX(Ratings,MATCH(Y31,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F31&lt;(INDEX(Ratings,MATCH(Y31,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R31" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S31" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R31" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S31" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T31" s="7"/>
@@ -5211,12 +5362,12 @@
       <c r="V31" s="7"/>
       <c r="W31" s="7"/>
       <c r="X31" s="7"/>
-      <c r="Y31" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z31" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="43"/>
       <c r="C32" s="44"/>
@@ -5234,15 +5385,26 @@
       <c r="O32" s="7"/>
       <c r="P32" s="7"/>
       <c r="Q32" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F32&gt;(INDEX(Ratings,MATCH(Y32,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F32&lt;(INDEX(Ratings,MATCH(Y32,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R32" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S32" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R32" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S32" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T32" s="7"/>
@@ -5250,12 +5412,12 @@
       <c r="V32" s="7"/>
       <c r="W32" s="7"/>
       <c r="X32" s="7"/>
-      <c r="Y32" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z32" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="45"/>
       <c r="C33" s="46"/>
@@ -5273,15 +5435,26 @@
       <c r="O33" s="7"/>
       <c r="P33" s="7"/>
       <c r="Q33" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F33&gt;(INDEX(Ratings,MATCH(Y33,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F33&lt;(INDEX(Ratings,MATCH(Y33,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R33" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S33" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R33" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S33" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T33" s="7"/>
@@ -5289,12 +5462,12 @@
       <c r="V33" s="7"/>
       <c r="W33" s="7"/>
       <c r="X33" s="7"/>
-      <c r="Y33" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z33" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="43"/>
       <c r="C34" s="44"/>
@@ -5312,15 +5485,26 @@
       <c r="O34" s="7"/>
       <c r="P34" s="7"/>
       <c r="Q34" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F34&gt;(INDEX(Ratings,MATCH(Y34,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F34&lt;(INDEX(Ratings,MATCH(Y34,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R34" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S34" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R34" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S34" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T34" s="7"/>
@@ -5328,12 +5512,12 @@
       <c r="V34" s="7"/>
       <c r="W34" s="7"/>
       <c r="X34" s="7"/>
-      <c r="Y34" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z34" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="45"/>
       <c r="C35" s="46"/>
@@ -5351,15 +5535,26 @@
       <c r="O35" s="7"/>
       <c r="P35" s="7"/>
       <c r="Q35" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F35&gt;(INDEX(Ratings,MATCH(Y35,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F35&lt;(INDEX(Ratings,MATCH(Y35,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R35" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S35" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R35" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S35" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T35" s="7"/>
@@ -5367,12 +5562,12 @@
       <c r="V35" s="7"/>
       <c r="W35" s="7"/>
       <c r="X35" s="7"/>
-      <c r="Y35" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z35" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="43"/>
       <c r="C36" s="44"/>
@@ -5390,15 +5585,26 @@
       <c r="O36" s="7"/>
       <c r="P36" s="7"/>
       <c r="Q36" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F36&gt;(INDEX(Ratings,MATCH(Y36,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F36&lt;(INDEX(Ratings,MATCH(Y36,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R36" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S36" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R36" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S36" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T36" s="7"/>
@@ -5406,12 +5612,12 @@
       <c r="V36" s="7"/>
       <c r="W36" s="7"/>
       <c r="X36" s="7"/>
-      <c r="Y36" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z36" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="45"/>
       <c r="C37" s="46"/>
@@ -5429,15 +5635,26 @@
       <c r="O37" s="7"/>
       <c r="P37" s="7"/>
       <c r="Q37" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F37&gt;(INDEX(Ratings,MATCH(Y37,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F37&lt;(INDEX(Ratings,MATCH(Y37,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R37" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S37" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R37" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S37" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T37" s="7"/>
@@ -5445,12 +5662,12 @@
       <c r="V37" s="7"/>
       <c r="W37" s="7"/>
       <c r="X37" s="7"/>
-      <c r="Y37" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z37" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="43"/>
       <c r="C38" s="44"/>
@@ -5468,15 +5685,26 @@
       <c r="O38" s="7"/>
       <c r="P38" s="7"/>
       <c r="Q38" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F38&gt;(INDEX(Ratings,MATCH(Y38,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F38&lt;(INDEX(Ratings,MATCH(Y38,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R38" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S38" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R38" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S38" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T38" s="7"/>
@@ -5484,12 +5712,12 @@
       <c r="V38" s="7"/>
       <c r="W38" s="7"/>
       <c r="X38" s="7"/>
-      <c r="Y38" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z38" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="45"/>
       <c r="C39" s="46"/>
@@ -5507,15 +5735,26 @@
       <c r="O39" s="7"/>
       <c r="P39" s="7"/>
       <c r="Q39" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F39&gt;(INDEX(Ratings,MATCH(Y39,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F39&lt;(INDEX(Ratings,MATCH(Y39,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R39" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S39" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R39" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S39" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T39" s="7"/>
@@ -5523,12 +5762,12 @@
       <c r="V39" s="7"/>
       <c r="W39" s="7"/>
       <c r="X39" s="7"/>
-      <c r="Y39" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z39" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="43"/>
       <c r="C40" s="44"/>
@@ -5546,15 +5785,26 @@
       <c r="O40" s="7"/>
       <c r="P40" s="7"/>
       <c r="Q40" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F40&gt;(INDEX(Ratings,MATCH(Y40,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F40&lt;(INDEX(Ratings,MATCH(Y40,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R40" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S40" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R40" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S40" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T40" s="7"/>
@@ -5562,12 +5812,12 @@
       <c r="V40" s="7"/>
       <c r="W40" s="7"/>
       <c r="X40" s="7"/>
-      <c r="Y40" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z40" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="45"/>
       <c r="C41" s="46"/>
@@ -5585,15 +5835,26 @@
       <c r="O41" s="7"/>
       <c r="P41" s="7"/>
       <c r="Q41" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F41&gt;(INDEX(Ratings,MATCH(Y41,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F41&lt;(INDEX(Ratings,MATCH(Y41,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R41" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S41" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R41" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S41" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T41" s="7"/>
@@ -5601,12 +5862,12 @@
       <c r="V41" s="7"/>
       <c r="W41" s="7"/>
       <c r="X41" s="7"/>
-      <c r="Y41" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z41" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="43"/>
       <c r="C42" s="44"/>
@@ -5624,15 +5885,26 @@
       <c r="O42" s="7"/>
       <c r="P42" s="7"/>
       <c r="Q42" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F42&gt;(INDEX(Ratings,MATCH(Y42,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F42&lt;(INDEX(Ratings,MATCH(Y42,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R42" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S42" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R42" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S42" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T42" s="7"/>
@@ -5640,12 +5912,12 @@
       <c r="V42" s="7"/>
       <c r="W42" s="7"/>
       <c r="X42" s="7"/>
-      <c r="Y42" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z42" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="45"/>
       <c r="C43" s="46"/>
@@ -5663,15 +5935,26 @@
       <c r="O43" s="7"/>
       <c r="P43" s="7"/>
       <c r="Q43" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F43&gt;(INDEX(Ratings,MATCH(Y43,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F43&lt;(INDEX(Ratings,MATCH(Y43,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R43" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S43" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R43" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S43" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T43" s="7"/>
@@ -5679,12 +5962,12 @@
       <c r="V43" s="7"/>
       <c r="W43" s="7"/>
       <c r="X43" s="7"/>
-      <c r="Y43" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z43" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="43"/>
       <c r="C44" s="44"/>
@@ -5702,15 +5985,26 @@
       <c r="O44" s="7"/>
       <c r="P44" s="7"/>
       <c r="Q44" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F44&gt;(INDEX(Ratings,MATCH(Y44,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F44&lt;(INDEX(Ratings,MATCH(Y44,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R44" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S44" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R44" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S44" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T44" s="7"/>
@@ -5718,12 +6012,12 @@
       <c r="V44" s="7"/>
       <c r="W44" s="7"/>
       <c r="X44" s="7"/>
-      <c r="Y44" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z44" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="45"/>
       <c r="C45" s="46"/>
@@ -5741,15 +6035,26 @@
       <c r="O45" s="7"/>
       <c r="P45" s="7"/>
       <c r="Q45" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F45&gt;(INDEX(Ratings,MATCH(Y45,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F45&lt;(INDEX(Ratings,MATCH(Y45,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R45" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S45" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R45" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S45" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T45" s="7"/>
@@ -5757,12 +6062,12 @@
       <c r="V45" s="7"/>
       <c r="W45" s="7"/>
       <c r="X45" s="7"/>
-      <c r="Y45" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z45" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="43"/>
       <c r="C46" s="44"/>
@@ -5780,15 +6085,26 @@
       <c r="O46" s="7"/>
       <c r="P46" s="7"/>
       <c r="Q46" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F46&gt;(INDEX(Ratings,MATCH(Y46,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F46&lt;(INDEX(Ratings,MATCH(Y46,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R46" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S46" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R46" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S46" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T46" s="7"/>
@@ -5796,12 +6112,12 @@
       <c r="V46" s="7"/>
       <c r="W46" s="7"/>
       <c r="X46" s="7"/>
-      <c r="Y46" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z46" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="45"/>
       <c r="C47" s="46"/>
@@ -5819,15 +6135,26 @@
       <c r="O47" s="7"/>
       <c r="P47" s="7"/>
       <c r="Q47" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F47&gt;(INDEX(Ratings,MATCH(Y47,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F47&lt;(INDEX(Ratings,MATCH(Y47,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R47" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S47" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R47" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S47" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T47" s="7"/>
@@ -5835,12 +6162,12 @@
       <c r="V47" s="7"/>
       <c r="W47" s="7"/>
       <c r="X47" s="7"/>
-      <c r="Y47" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z47" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="43"/>
       <c r="C48" s="44"/>
@@ -5858,15 +6185,26 @@
       <c r="O48" s="7"/>
       <c r="P48" s="7"/>
       <c r="Q48" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F48&gt;(INDEX(Ratings,MATCH(Y48,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F48&lt;(INDEX(Ratings,MATCH(Y48,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R48" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S48" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R48" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S48" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T48" s="7"/>
@@ -5874,12 +6212,12 @@
       <c r="V48" s="7"/>
       <c r="W48" s="7"/>
       <c r="X48" s="7"/>
-      <c r="Y48" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z48" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:26" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="45"/>
       <c r="C49" s="46"/>
@@ -5897,15 +6235,26 @@
       <c r="O49" s="7"/>
       <c r="P49" s="7"/>
       <c r="Q49" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F49&gt;(INDEX(Ratings,MATCH(Y49,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F49&lt;(INDEX(Ratings,MATCH(Y49,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R49" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S49" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R49" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S49" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T49" s="7"/>
@@ -5913,12 +6262,12 @@
       <c r="V49" s="7"/>
       <c r="W49" s="7"/>
       <c r="X49" s="7"/>
-      <c r="Y49" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z49" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:25" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:26" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="8"/>
       <c r="B50" s="47"/>
       <c r="C50" s="48"/>
@@ -5936,15 +6285,26 @@
       <c r="O50" s="8"/>
       <c r="P50" s="8"/>
       <c r="Q50" s="7" t="e">
+        <f>IF(
+    AND(
+        OR(
+             AND(BACKLAY="BACK",(F50&gt;(INDEX(Ratings,MATCH(Y50,SelectionID,0))))),
+             AND(BACKLAY="LAY",(F50&lt;(INDEX(Ratings,MATCH(Y50,SelectionID,0)))))),
+        Overround&lt;UserOverround,
+        TimeTillJump&lt;UserTimeTillJump,
+         InPlay="Not In Play",
+        MarketStatus&lt;&gt;"Suspended"),
+        BACKLAY,
+    ""
+)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="R50" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="S50" s="81" t="str">
         <f t="shared" si="0"/>
-        <v>#N/A</v>
-      </c>
-      <c r="R50" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="S50" s="81" t="str">
-        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="T50" s="8"/>
@@ -5952,8 +6312,8 @@
       <c r="V50" s="8"/>
       <c r="W50" s="8"/>
       <c r="X50" s="8"/>
-      <c r="Y50" s="19" t="str">
-        <f t="shared" si="2"/>
+      <c r="Z50" s="19" t="str">
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5972,7 +6332,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:Y9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -6040,11 +6400,11 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>535</v>
+        <v>524</v>
       </c>
       <c r="C9" s="3">
         <f>IF(LEFT(Market!D2)&lt;&gt;"-",(HOUR(Market!$D$2)*3600)+(MINUTE(Market!$D$2)*60)+SECOND(Market!$D$2),-((HOUR(SUBSTITUTE(Market!$D$2,"-",""))*3600)+(MINUTE(SUBSTITUTE(Market!$D$2,"-",""))*60)+SECOND(SUBSTITUTE(Market!$D$2,"-",""))))</f>
-        <v>662</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -6066,7 +6426,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>